<commit_message>
Req column 3 player game actions
</commit_message>
<xml_diff>
--- a/docs/3 player game actions and chat manual test.xlsx
+++ b/docs/3 player game actions and chat manual test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimi\OneDrive\Documents\Courses\Fundamental of SWE\3310 Group project\cse3310_sp24_group_12\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271F2910-9B4F-5E47-B6A9-E30FA3253412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F102393F-86FB-4D1A-B05E-CD2E01AB113A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="14000" windowHeight="16500" xr2:uid="{E84A72F2-B4C3-BF4C-A5CC-83B084D2C238}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E84A72F2-B4C3-BF4C-A5CC-83B084D2C238}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Action</t>
   </si>
@@ -192,13 +192,34 @@
   </si>
   <si>
     <t>Players are taken to leaderboard scrren but scores are not provided and no other action is available. Stuck</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>SREQ002</t>
+  </si>
+  <si>
+    <t>SREQ004</t>
+  </si>
+  <si>
+    <t>SREQ009</t>
+  </si>
+  <si>
+    <t>SREQ039</t>
+  </si>
+  <si>
+    <t>SREQ026</t>
+  </si>
+  <si>
+    <t>SREQ041</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,17 +303,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,83 +649,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6B3E84-021E-9E47-B26F-F97D8577B605}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="I7" sqref="I7:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -717,14 +758,14 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -733,80 +774,100 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -819,14 +880,14 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -835,80 +896,100 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -921,14 +1002,14 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -937,114 +1018,144 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6" t="s">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1063,8 +1174,14 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1077,280 +1194,364 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.95" customHeight="1">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6" t="s">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6" t="s">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.95" customHeight="1">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6" t="s">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6" t="s">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6" t="s">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.95" customHeight="1">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6" t="s">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.95" customHeight="1">
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+    </row>
+    <row r="41" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6" t="s">
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1370,7 +1571,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1384,7 +1585,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -1404,7 +1605,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1418,7 +1619,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -1438,7 +1639,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1452,75 +1653,95 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6" t="s">
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6" t="s">
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1535,25 +1756,71 @@
       <c r="L53" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="78">
-    <mergeCell ref="I47:L48"/>
-    <mergeCell ref="I51:L52"/>
-    <mergeCell ref="I49:L50"/>
-    <mergeCell ref="I25:L26"/>
-    <mergeCell ref="I31:L32"/>
-    <mergeCell ref="I37:L38"/>
-    <mergeCell ref="I27:L28"/>
-    <mergeCell ref="I33:L34"/>
-    <mergeCell ref="I39:L40"/>
-    <mergeCell ref="I41:L42"/>
-    <mergeCell ref="I43:L44"/>
-    <mergeCell ref="I45:L46"/>
-    <mergeCell ref="I35:L36"/>
-    <mergeCell ref="I17:L18"/>
-    <mergeCell ref="I19:L20"/>
-    <mergeCell ref="I21:L22"/>
-    <mergeCell ref="I23:L24"/>
-    <mergeCell ref="I29:L30"/>
+  <mergeCells count="98">
+    <mergeCell ref="M51:P52"/>
+    <mergeCell ref="M35:P36"/>
+    <mergeCell ref="M37:P38"/>
+    <mergeCell ref="M39:P40"/>
+    <mergeCell ref="M41:P42"/>
+    <mergeCell ref="M49:P50"/>
+    <mergeCell ref="M25:P26"/>
+    <mergeCell ref="M27:P28"/>
+    <mergeCell ref="M29:P30"/>
+    <mergeCell ref="M31:P32"/>
+    <mergeCell ref="M33:P34"/>
+    <mergeCell ref="M15:P16"/>
+    <mergeCell ref="M19:P20"/>
+    <mergeCell ref="M21:P22"/>
+    <mergeCell ref="M23:P24"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="M9:P10"/>
+    <mergeCell ref="M13:P14"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A5:D6"/>
+    <mergeCell ref="A31:D32"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="A19:D20"/>
+    <mergeCell ref="A21:D22"/>
+    <mergeCell ref="A23:D24"/>
+    <mergeCell ref="A25:D26"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="A45:D46"/>
+    <mergeCell ref="A47:D48"/>
+    <mergeCell ref="A49:D50"/>
+    <mergeCell ref="A51:D52"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="E5:H6"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="E11:H12"/>
+    <mergeCell ref="E13:H14"/>
+    <mergeCell ref="A33:D34"/>
+    <mergeCell ref="A35:D36"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="A39:D40"/>
+    <mergeCell ref="A41:D42"/>
+    <mergeCell ref="A43:D44"/>
+    <mergeCell ref="E33:H34"/>
+    <mergeCell ref="E39:H40"/>
+    <mergeCell ref="E41:H42"/>
+    <mergeCell ref="E43:H44"/>
+    <mergeCell ref="E15:H16"/>
+    <mergeCell ref="E17:H18"/>
+    <mergeCell ref="E19:H20"/>
+    <mergeCell ref="E21:H22"/>
+    <mergeCell ref="E23:H24"/>
+    <mergeCell ref="E29:H30"/>
     <mergeCell ref="E45:H46"/>
     <mergeCell ref="E47:H48"/>
     <mergeCell ref="E51:H52"/>
@@ -1570,50 +1837,24 @@
     <mergeCell ref="E31:H32"/>
     <mergeCell ref="E37:H38"/>
     <mergeCell ref="E27:H28"/>
-    <mergeCell ref="E33:H34"/>
-    <mergeCell ref="E39:H40"/>
-    <mergeCell ref="E41:H42"/>
-    <mergeCell ref="E43:H44"/>
-    <mergeCell ref="E15:H16"/>
-    <mergeCell ref="E17:H18"/>
-    <mergeCell ref="E19:H20"/>
-    <mergeCell ref="E21:H22"/>
-    <mergeCell ref="E23:H24"/>
-    <mergeCell ref="E29:H30"/>
-    <mergeCell ref="A45:D46"/>
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="A49:D50"/>
-    <mergeCell ref="A51:D52"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="E5:H6"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="E9:H10"/>
-    <mergeCell ref="E11:H12"/>
-    <mergeCell ref="E13:H14"/>
-    <mergeCell ref="A33:D34"/>
-    <mergeCell ref="A35:D36"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="A39:D40"/>
-    <mergeCell ref="A41:D42"/>
-    <mergeCell ref="A43:D44"/>
-    <mergeCell ref="A31:D32"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="A11:D12"/>
-    <mergeCell ref="A13:D14"/>
-    <mergeCell ref="A15:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="A19:D20"/>
-    <mergeCell ref="A21:D22"/>
-    <mergeCell ref="A23:D24"/>
-    <mergeCell ref="A25:D26"/>
-    <mergeCell ref="A27:D28"/>
-    <mergeCell ref="A29:D30"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="I1:L2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="A5:D6"/>
+    <mergeCell ref="I17:L18"/>
+    <mergeCell ref="I19:L20"/>
+    <mergeCell ref="I21:L22"/>
+    <mergeCell ref="I23:L24"/>
+    <mergeCell ref="I29:L30"/>
+    <mergeCell ref="I47:L48"/>
+    <mergeCell ref="I51:L52"/>
+    <mergeCell ref="I49:L50"/>
+    <mergeCell ref="I25:L26"/>
+    <mergeCell ref="I31:L32"/>
+    <mergeCell ref="I37:L38"/>
+    <mergeCell ref="I27:L28"/>
+    <mergeCell ref="I33:L34"/>
+    <mergeCell ref="I39:L40"/>
+    <mergeCell ref="I41:L42"/>
+    <mergeCell ref="I43:L44"/>
+    <mergeCell ref="I45:L46"/>
+    <mergeCell ref="I35:L36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>